<commit_message>
added shortcuts, and added hi-lock keybindings
</commit_message>
<xml_diff>
--- a/emacs_shortcuts.xlsx
+++ b/emacs_shortcuts.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="19230" windowHeight="8280"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="19230" windowHeight="8280" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="emacs shortcuts" sheetId="1" r:id="rId1"/>
     <sheet name="org-ref" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="macro" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Time">'org-ref'!$E$9</definedName>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="640">
   <si>
     <t>Function</t>
   </si>
@@ -2353,6 +2354,18 @@
   </si>
   <si>
     <t xml:space="preserve">         ("C-h w" . helm-descbinds)))</t>
+  </si>
+  <si>
+    <t>Set initial counter value (before macro recording starts)</t>
+  </si>
+  <si>
+    <t>c-x c-k c-c</t>
+  </si>
+  <si>
+    <t>insert a counter</t>
+  </si>
+  <si>
+    <t>c-x c-k c-i</t>
   </si>
 </sst>
 </file>
@@ -2839,7 +2852,7 @@
   </sheetPr>
   <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B79" sqref="B79:B80"/>
     </sheetView>
   </sheetViews>
@@ -4007,7 +4020,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="E44" s="15" t="s">
         <v>548</v>
       </c>
@@ -6424,9 +6437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6540,4 +6551,38 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>636</v>
+      </c>
+      <c r="B1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>638</v>
+      </c>
+      <c r="B2" t="s">
+        <v>639</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
minor changes. got smart compile back on F12
</commit_message>
<xml_diff>
--- a/emacs_shortcuts.xlsx
+++ b/emacs_shortcuts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="19230" windowHeight="8280" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="19230" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="emacs shortcuts" sheetId="1" r:id="rId1"/>
@@ -2852,8 +2852,8 @@
   </sheetPr>
   <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79:B80"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4020,7 +4020,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E44" s="15" t="s">
         <v>548</v>
       </c>
@@ -6557,7 +6557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>